<commit_message>
Kundenverwaltung inkludiert (muss noch angepasst werden) CustomerService fast fertig, MVC Implementiert für meine Klassen, Unternehmen kann jetzt verwaltet werden
</commit_message>
<xml_diff>
--- a/Entwuerfe/2018_01_24 Ein- und Ausgabe.xlsx
+++ b/Entwuerfe/2018_01_24 Ein- und Ausgabe.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Eingabe:</t>
   </si>
@@ -74,7 +74,40 @@
     <t>gesamtpreis</t>
   </si>
   <si>
-    <t xml:space="preserve">kundennummer vorname </t>
+    <t xml:space="preserve">kundennummer </t>
+  </si>
+  <si>
+    <t>vorname</t>
+  </si>
+  <si>
+    <t>nachname</t>
+  </si>
+  <si>
+    <t>straße hausnummer</t>
+  </si>
+  <si>
+    <t>plz ort</t>
+  </si>
+  <si>
+    <t>straße</t>
+  </si>
+  <si>
+    <t>plz</t>
+  </si>
+  <si>
+    <t>ort</t>
+  </si>
+  <si>
+    <t>ort,</t>
+  </si>
+  <si>
+    <t>firmenname,</t>
+  </si>
+  <si>
+    <t>hausnummer,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> den datum</t>
   </si>
 </sst>
 </file>
@@ -114,7 +147,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -122,14 +155,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -462,50 +505,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>4</v>
       </c>
@@ -541,7 +628,7 @@
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -551,7 +638,7 @@
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>